<commit_message>
adress xa huyen tinh
</commit_message>
<xml_diff>
--- a/PetSusan/script/file/rate.xlsx
+++ b/PetSusan/script/file/rate.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hoang\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\petsusan\PetSusan\script\file\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -345,7 +345,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C939"/>
   <sheetViews>
-    <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" topLeftCell="A914" workbookViewId="0"/>
+    <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>